<commit_message>
MechaBible Mark I: Programming - Python: Arduino GUI Multiple Windows, Database Connection & Data Analysis
</commit_message>
<xml_diff>
--- a/1.-Data Science/0.-Archivos_Ejercicios_Python/23.-GUI PyQt5 Conexion DataBase/23.-Reporte Analisis de Datos 2.xlsx
+++ b/1.-Data Science/0.-Archivos_Ejercicios_Python/23.-GUI PyQt5 Conexion DataBase/23.-Reporte Analisis de Datos 2.xlsx
@@ -14,7 +14,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+  <si>
+    <t>Title A1.1</t>
+  </si>
+  <si>
+    <t>Static Row 1</t>
+  </si>
+  <si>
+    <t>Static Row 2</t>
+  </si>
+  <si>
+    <t>Static Row 3</t>
+  </si>
+  <si>
+    <t>Static Row 4</t>
+  </si>
+  <si>
+    <t>Static Row 5</t>
+  </si>
+  <si>
+    <t>Static Row 6</t>
+  </si>
+  <si>
+    <t>Title A1.2</t>
+  </si>
+  <si>
+    <t>Title A1.3</t>
+  </si>
   <si>
     <t>Titulo Static</t>
   </si>
@@ -80,6 +107,54 @@
   </si>
   <si>
     <t>01-12-2023</t>
+  </si>
+  <si>
+    <t>Title A2</t>
+  </si>
+  <si>
+    <t>Subtitle A2.1</t>
+  </si>
+  <si>
+    <t>Subtitle A2.2</t>
+  </si>
+  <si>
+    <t>Subtitle A2.3</t>
+  </si>
+  <si>
+    <t>Static Text: Lorem ipsum dolor sit amet, consectetur adipiscing elit. Quisque non laoreet mauris. Pellentesque habitant morbi tristique senectus et netus et malesuada fames ac turpis egestas. Curabitur vulputate bibendum nibh elementum pulvinar. Integer a leo in orci ultricies fermentum. Ut vitae velit et sapien congue accumsan sed tincidunt dui. Ut elementum imperdiet nunc, non hendrerit enim ultrices at. Sed rhoncus vehicula.</t>
+  </si>
+  <si>
+    <t>Title B1</t>
+  </si>
+  <si>
+    <t>Title B1.1</t>
+  </si>
+  <si>
+    <t>Subtitle 1</t>
+  </si>
+  <si>
+    <t>Static Row 7</t>
+  </si>
+  <si>
+    <t>Subtitle 2</t>
+  </si>
+  <si>
+    <t>Title B1.2</t>
+  </si>
+  <si>
+    <t>Title B1.3</t>
+  </si>
+  <si>
+    <t>Title B1.4</t>
+  </si>
+  <si>
+    <t>Title B1.5</t>
+  </si>
+  <si>
+    <t>Title B1.6</t>
+  </si>
+  <si>
+    <t>Title B1.7</t>
   </si>
 </sst>
 </file>
@@ -466,129 +541,288 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
-        <v>21</v>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>